<commit_message>
delete unneeded cells, add simple version for current usage
</commit_message>
<xml_diff>
--- a/data_rand_num.xlsx
+++ b/data_rand_num.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/therese/Sigman Group Dropbox/Therese Wild/merck_collab/clustering_gs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B03E684-0BAF-774B-AFB7-B922635AD131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B27284D-EB09-A04D-BE7D-C358EE6DCA79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="760" windowWidth="16100" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>id</t>
   </si>
@@ -152,6 +152,12 @@
   </si>
   <si>
     <t>error</t>
+  </si>
+  <si>
+    <t>arbr144</t>
+  </si>
+  <si>
+    <t>BrC1=CC=CC=C1</t>
   </si>
 </sst>
 </file>
@@ -519,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -693,452 +699,463 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
         <v>42</v>
       </c>
-      <c r="D5">
-        <v>3.9233801184838102E-2</v>
-      </c>
-      <c r="E5">
-        <v>0.59434879809960717</v>
-      </c>
-      <c r="F5">
-        <v>0.45821571439947978</v>
-      </c>
-      <c r="G5">
-        <v>0.99182792633404548</v>
-      </c>
-      <c r="H5">
-        <v>0.88864594574476197</v>
-      </c>
-      <c r="I5">
-        <v>0.35409623518933969</v>
-      </c>
-      <c r="J5">
-        <v>0.72274184879366965</v>
-      </c>
-      <c r="K5">
-        <v>0.44183153744103187</v>
-      </c>
-      <c r="L5">
-        <v>0.69697416029529891</v>
-      </c>
-      <c r="M5">
-        <v>0.63302626562404496</v>
-      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
         <v>42</v>
       </c>
       <c r="D6">
-        <v>4.0811064251796918E-2</v>
+        <v>3.9233801184838102E-2</v>
       </c>
       <c r="E6">
-        <v>0.47558212315498188</v>
+        <v>0.59434879809960717</v>
       </c>
       <c r="F6">
-        <v>0.49133526471647038</v>
+        <v>0.45821571439947978</v>
       </c>
       <c r="G6">
-        <v>0.9149047565562356</v>
+        <v>0.99182792633404548</v>
       </c>
       <c r="H6">
-        <v>0.38591860459793831</v>
+        <v>0.88864594574476197</v>
       </c>
       <c r="I6">
-        <v>0.17485849518231131</v>
+        <v>0.35409623518933969</v>
       </c>
       <c r="J6">
-        <v>0.1035818589050892</v>
+        <v>0.72274184879366965</v>
       </c>
       <c r="K6">
-        <v>0.1599644915867878</v>
+        <v>0.44183153744103187</v>
       </c>
       <c r="L6">
-        <v>0.41634525736718941</v>
+        <v>0.69697416029529891</v>
       </c>
       <c r="M6">
-        <v>4.7376117105064508E-2</v>
+        <v>0.63302626562404496</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
         <v>42</v>
       </c>
       <c r="D7">
-        <v>0.95503897280132188</v>
+        <v>4.0811064251796918E-2</v>
       </c>
       <c r="E7">
-        <v>2.126808917388268E-2</v>
+        <v>0.47558212315498188</v>
       </c>
       <c r="F7">
-        <v>0.42701636374115493</v>
+        <v>0.49133526471647038</v>
       </c>
       <c r="G7">
-        <v>0.24485341847771699</v>
+        <v>0.9149047565562356</v>
       </c>
       <c r="H7">
-        <v>0.27546282706620961</v>
+        <v>0.38591860459793831</v>
       </c>
       <c r="I7">
-        <v>0.123705975226871</v>
+        <v>0.17485849518231131</v>
       </c>
       <c r="J7">
-        <v>0.29669111412034421</v>
+        <v>0.1035818589050892</v>
       </c>
       <c r="K7">
-        <v>0.94093383233720573</v>
+        <v>0.1599644915867878</v>
       </c>
       <c r="L7">
-        <v>0.83584133363106616</v>
+        <v>0.41634525736718941</v>
       </c>
       <c r="M7">
-        <v>0.39295612285191511</v>
+        <v>4.7376117105064508E-2</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D8">
-        <v>0.13845040694181279</v>
+        <v>0.95503897280132188</v>
       </c>
       <c r="E8">
-        <v>0.88093784766393501</v>
+        <v>2.126808917388268E-2</v>
       </c>
       <c r="F8">
-        <v>0.16739245239331141</v>
+        <v>0.42701636374115493</v>
       </c>
       <c r="G8">
-        <v>0.88937895539908973</v>
+        <v>0.24485341847771699</v>
       </c>
       <c r="H8">
-        <v>0.89815480974480066</v>
+        <v>0.27546282706620961</v>
       </c>
       <c r="I8">
-        <v>0.380557816841954</v>
+        <v>0.123705975226871</v>
       </c>
       <c r="J8">
-        <v>0.90221387122652019</v>
+        <v>0.29669111412034421</v>
       </c>
       <c r="K8">
-        <v>0.74897195560551988</v>
+        <v>0.94093383233720573</v>
       </c>
       <c r="L8">
-        <v>0.6093816208075189</v>
+        <v>0.83584133363106616</v>
       </c>
       <c r="M8">
-        <v>0.5289630937872607</v>
+        <v>0.39295612285191511</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
         <v>41</v>
       </c>
       <c r="D9">
-        <v>0.66979245388834152</v>
+        <v>0.13845040694181279</v>
       </c>
       <c r="E9">
-        <v>0.67372399565053942</v>
+        <v>0.88093784766393501</v>
       </c>
       <c r="F9">
-        <v>0.32961206419296463</v>
+        <v>0.16739245239331141</v>
       </c>
       <c r="G9">
-        <v>9.360075565001813E-2</v>
+        <v>0.88937895539908973</v>
       </c>
       <c r="H9">
-        <v>0.72305194775380621</v>
+        <v>0.89815480974480066</v>
       </c>
       <c r="I9">
-        <v>7.3801183749372834E-2</v>
+        <v>0.380557816841954</v>
       </c>
       <c r="J9">
-        <v>3.6201428291025912E-2</v>
+        <v>0.90221387122652019</v>
       </c>
       <c r="K9">
-        <v>0.97023741043539002</v>
+        <v>0.74897195560551988</v>
       </c>
       <c r="L9">
-        <v>0.38644740545750011</v>
+        <v>0.6093816208075189</v>
       </c>
       <c r="M9">
-        <v>0.60148204700901187</v>
+        <v>0.5289630937872607</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
         <v>41</v>
       </c>
       <c r="D10">
-        <v>0.94210958437967107</v>
+        <v>0.66979245388834152</v>
       </c>
       <c r="E10">
-        <v>0.36954588799559768</v>
+        <v>0.67372399565053942</v>
       </c>
       <c r="F10">
-        <v>0.35336509583212322</v>
+        <v>0.32961206419296463</v>
       </c>
       <c r="G10">
-        <v>0.85168295578540421</v>
+        <v>9.360075565001813E-2</v>
       </c>
       <c r="H10">
-        <v>0.118317040715418</v>
+        <v>0.72305194775380621</v>
       </c>
       <c r="I10">
-        <v>0.38794898061000122</v>
+        <v>7.3801183749372834E-2</v>
       </c>
       <c r="J10">
-        <v>0.29779880888292298</v>
+        <v>3.6201428291025912E-2</v>
       </c>
       <c r="K10">
-        <v>0.37501030110022782</v>
+        <v>0.97023741043539002</v>
       </c>
       <c r="L10">
-        <v>0.75860245105532409</v>
+        <v>0.38644740545750011</v>
       </c>
       <c r="M10">
-        <v>0.18379411509316951</v>
+        <v>0.60148204700901187</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
         <v>41</v>
       </c>
       <c r="D11">
-        <v>0.30352671499086581</v>
+        <v>0.94210958437967107</v>
       </c>
       <c r="E11">
-        <v>0.59817777853291654</v>
+        <v>0.36954588799559768</v>
       </c>
       <c r="F11">
-        <v>0.72435545193006601</v>
+        <v>0.35336509583212322</v>
       </c>
       <c r="G11">
-        <v>0.51306468587773013</v>
+        <v>0.85168295578540421</v>
       </c>
       <c r="H11">
-        <v>0.34791981922533088</v>
+        <v>0.118317040715418</v>
       </c>
       <c r="I11">
-        <v>0.67177465097282885</v>
+        <v>0.38794898061000122</v>
       </c>
       <c r="J11">
-        <v>0.88311323654450002</v>
+        <v>0.29779880888292298</v>
       </c>
       <c r="K11">
-        <v>0.68389549764384661</v>
+        <v>0.37501030110022782</v>
       </c>
       <c r="L11">
-        <v>0.38467406828075562</v>
+        <v>0.75860245105532409</v>
       </c>
       <c r="M11">
-        <v>0.65200690374850068</v>
+        <v>0.18379411509316951</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D12">
-        <v>0.82280606540341084</v>
+        <v>0.30352671499086581</v>
       </c>
       <c r="E12">
-        <v>0.97145963222884824</v>
+        <v>0.59817777853291654</v>
       </c>
       <c r="F12">
-        <v>0.77397884491813329</v>
+        <v>0.72435545193006601</v>
       </c>
       <c r="G12">
-        <v>0.63933696493838721</v>
+        <v>0.51306468587773013</v>
       </c>
       <c r="H12">
-        <v>0.32944727889970332</v>
+        <v>0.34791981922533088</v>
       </c>
       <c r="I12">
-        <v>8.4099649683441746E-2</v>
+        <v>0.67177465097282885</v>
       </c>
       <c r="J12">
-        <v>0.78308857369563623</v>
+        <v>0.88311323654450002</v>
       </c>
       <c r="K12">
-        <v>0.40223352342110991</v>
+        <v>0.68389549764384661</v>
       </c>
       <c r="L12">
-        <v>0.7226314678970136</v>
+        <v>0.38467406828075562</v>
       </c>
       <c r="M12">
-        <v>5.4973327262096583E-2</v>
+        <v>0.65200690374850068</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D13">
-        <v>0.71689486698991167</v>
+        <v>0.82280606540341084</v>
       </c>
       <c r="E13">
-        <v>0.83214416591774643</v>
+        <v>0.97145963222884824</v>
       </c>
       <c r="F13">
-        <v>0.53885524124041217</v>
+        <v>0.77397884491813329</v>
       </c>
       <c r="G13">
-        <v>0.31206939607351719</v>
+        <v>0.63933696493838721</v>
       </c>
       <c r="H13">
-        <v>6.5106790816691906E-2</v>
+        <v>0.32944727889970332</v>
       </c>
       <c r="I13">
-        <v>0.89964661118690781</v>
+        <v>8.4099649683441746E-2</v>
       </c>
       <c r="J13">
-        <v>4.8726660644639597E-2</v>
+        <v>0.78308857369563623</v>
       </c>
       <c r="K13">
-        <v>0.61805306195536569</v>
+        <v>0.40223352342110991</v>
       </c>
       <c r="L13">
-        <v>0.65533659489528384</v>
+        <v>0.7226314678970136</v>
       </c>
       <c r="M13">
-        <v>0.97271080125028364</v>
+        <v>5.4973327262096583E-2</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
         <v>41</v>
       </c>
       <c r="D14">
-        <v>0.7818223351174528</v>
+        <v>0.71689486698991167</v>
       </c>
       <c r="E14">
-        <v>2.0020491172982099E-2</v>
+        <v>0.83214416591774643</v>
       </c>
       <c r="F14">
-        <v>0.55874922367376145</v>
+        <v>0.53885524124041217</v>
       </c>
       <c r="G14">
-        <v>0.1852904660508988</v>
+        <v>0.31206939607351719</v>
       </c>
       <c r="H14">
-        <v>0.90624523103929688</v>
+        <v>6.5106790816691906E-2</v>
       </c>
       <c r="I14">
-        <v>0.2067874361873038</v>
+        <v>0.89964661118690781</v>
       </c>
       <c r="J14">
-        <v>0.37676375018919023</v>
+        <v>4.8726660644639597E-2</v>
       </c>
       <c r="K14">
-        <v>0.55702904791135821</v>
+        <v>0.61805306195536569</v>
       </c>
       <c r="L14">
-        <v>0.2128350222930315</v>
+        <v>0.65533659489528384</v>
       </c>
       <c r="M14">
-        <v>0.25608294626890571</v>
+        <v>0.97271080125028364</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
         <v>41</v>
       </c>
       <c r="D15">
+        <v>0.7818223351174528</v>
+      </c>
+      <c r="E15">
+        <v>2.0020491172982099E-2</v>
+      </c>
+      <c r="F15">
+        <v>0.55874922367376145</v>
+      </c>
+      <c r="G15">
+        <v>0.1852904660508988</v>
+      </c>
+      <c r="H15">
+        <v>0.90624523103929688</v>
+      </c>
+      <c r="I15">
+        <v>0.2067874361873038</v>
+      </c>
+      <c r="J15">
+        <v>0.37676375018919023</v>
+      </c>
+      <c r="K15">
+        <v>0.55702904791135821</v>
+      </c>
+      <c r="L15">
+        <v>0.2128350222930315</v>
+      </c>
+      <c r="M15">
+        <v>0.25608294626890571</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16">
         <v>0.83874510385396417</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <v>0.79081160509419934</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <v>0.2465855447090145</v>
       </c>
-      <c r="G15">
+      <c r="G16">
         <v>0.46413145211994111</v>
       </c>
-      <c r="H15">
+      <c r="H16">
         <v>0.1907144569540086</v>
       </c>
-      <c r="I15">
+      <c r="I16">
         <v>0.98478019172199271</v>
       </c>
-      <c r="J15">
+      <c r="J16">
         <v>0.70570370449627506</v>
       </c>
-      <c r="K15">
+      <c r="K16">
         <v>9.4927570388136817E-2</v>
       </c>
-      <c r="L15">
+      <c r="L16">
         <v>0.62391020092090788</v>
       </c>
-      <c r="M15">
+      <c r="M16">
         <v>0.19341675212779461</v>
       </c>
     </row>

</xml_diff>